<commit_message>
Refactoring and starting with with genetic refactoring for metrics implementation.
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.01999831199645996</v>
+        <v>0.06229925155639648</v>
       </c>
     </row>
     <row r="7">
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.19100022315979</v>
+        <v>0.2040002346038818</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.09400129318237305</v>
+        <v>0.1429991722106934</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All strategies are returning the oh well known small phi, congrats man! Good work, let's keep it rolling!
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -473,12 +473,12 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>- - -</t>
+          <t>╌╌╌╌╌╌╌</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>- - -</t>
+          <t>╌╌╌╌╌╌╌</t>
         </is>
       </c>
     </row>
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.06229925155639648</v>
+        <v>0.06800341606140137</v>
       </c>
     </row>
     <row r="7">
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2040002346038818</v>
+        <v>0.2119014263153076</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1429991722106934</v>
+        <v>0.145902156829834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All Strategies endpoint now has the genetic strategy, but isn't perfect...
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -473,43 +473,63 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>╌╌╌╌╌╌╌</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>╌╌╌╌╌╌╌</t>
-        </is>
+          <t>φ Genético</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>(ms) PyPhi</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.06800341606140137</v>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>(ms) Fuerza Brutal</t>
+          <t>(ms) PyPhi</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2119014263153076</v>
+        <v>0.06499814987182617</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
+          <t>(ms) Fuerza Brutal</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>0.1985921859741211</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
           <t>(ms) Ramificación</t>
         </is>
       </c>
-      <c r="B8" t="n">
-        <v>0.145902156829834</v>
+      <c r="B9" t="n">
+        <v>0.1363875865936279</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>(ms) Genético</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.7495453357696533</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Important improvement over the parameter passing but, genetic should have a even better way.
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -499,7 +499,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.06499814987182617</v>
+        <v>0.05704092979431152</v>
       </c>
     </row>
     <row r="8">
@@ -509,7 +509,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1985921859741211</v>
+        <v>0.2069904804229736</v>
       </c>
     </row>
     <row r="9">
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1363875865936279</v>
+        <v>0.1339104175567627</v>
       </c>
     </row>
     <row r="10">
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.7495453357696533</v>
+        <v>0.2220222949981689</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Is practically functionall the merge of the dataframes.
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Red 5 Nodos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Multiple Metrics" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,6 +439,36 @@
           <t>11100=(11111|11111)</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>11100=(11111|11111)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>11010=(11100|11100)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>11100=(11111|11111)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>11010=(11100|11100)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>11100=(11111|11111)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>11010=(11100|11100)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -447,8 +477,20 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
-      </c>
+        <v>0.25</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -457,6 +499,24 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -467,6 +527,24 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -477,6 +555,24 @@
         </is>
       </c>
       <c r="B5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -491,6 +587,36 @@
           <t>═━━━━━═</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -499,8 +625,20 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.05296802520751953</v>
-      </c>
+        <v>0.09630870819091797</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.03001594543457031</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.02126073837280273</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>0.01906681060791016</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -509,7 +647,25 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2013640403747559</v>
+        <v>0.2383427619934082</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2321922779083252</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0.03448390960693359</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.2031698226928711</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.03514933586120605</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.1948869228363037</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.03464770317077637</v>
       </c>
     </row>
     <row r="9">
@@ -519,7 +675,25 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1332182884216309</v>
+        <v>0.1576423645019531</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1008610725402832</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0385594367980957</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.1576919555664062</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0370633602142334</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.09760618209838867</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.03594970703125</v>
       </c>
     </row>
     <row r="10">
@@ -529,7 +703,25 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3390843868255615</v>
+        <v>0.8599867820739746</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.1246757507324219</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.05199742317199707</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.1527853012084961</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.05016684532165527</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.1371281147003174</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.04836392402648926</v>
       </c>
     </row>
     <row r="11">
@@ -539,6 +731,36 @@
         </is>
       </c>
       <c r="B11" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
         <is>
           <t>═━━━━━═</t>
         </is>

</xml_diff>

<commit_message>
Now works semi-properly the reports module, but is showable, noice.
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,32 +441,17 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>00111=(11011|11101)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>11100=(11111|11111)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>11010=(11100|11100)</t>
-        </is>
-      </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>11100=(11111|11111)</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>11010=(11100|11100)</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>11100=(11111|11111)</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>11010=(11100|11100)</t>
+          <t>00111=(11011|11101)</t>
         </is>
       </c>
     </row>
@@ -479,18 +464,11 @@
       <c r="B2" t="n">
         <v>0.25</v>
       </c>
-      <c r="C2" t="n">
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="n">
         <v>0.25</v>
       </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="H2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -502,21 +480,12 @@
         <v>0.25</v>
       </c>
       <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.25</v>
       </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
       <c r="E3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="H3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -530,21 +499,12 @@
         <v>0.25</v>
       </c>
       <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.25</v>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
       <c r="E4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="H4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -555,24 +515,15 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" t="n">
         <v>0</v>
       </c>
     </row>
@@ -602,21 +553,6 @@
           <t>═━━━━━═</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>═━━━━━═</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>═━━━━━═</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>═━━━━━═</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -625,20 +561,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.09630870819091797</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0.03001594543457031</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="n">
-        <v>0.02126073837280273</v>
-      </c>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="n">
-        <v>0.01906681060791016</v>
-      </c>
-      <c r="H7" t="inlineStr"/>
+        <v>0.01952672004699707</v>
+      </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="n">
+        <v>0.02027297019958496</v>
+      </c>
+      <c r="E7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -647,25 +576,16 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2383427619934082</v>
+        <v>0.2005040645599365</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2321922779083252</v>
+        <v>0.03600215911865234</v>
       </c>
       <c r="D8" t="n">
-        <v>0.03448390960693359</v>
+        <v>0.1984729766845703</v>
       </c>
       <c r="E8" t="n">
-        <v>0.2031698226928711</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0.03514933586120605</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0.1948869228363037</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.03464770317077637</v>
+        <v>0.0342252254486084</v>
       </c>
     </row>
     <row r="9">
@@ -675,25 +595,16 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.1576423645019531</v>
+        <v>0.09668254852294922</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1008610725402832</v>
+        <v>0.03748154640197754</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0385594367980957</v>
+        <v>0.09663057327270508</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1576919555664062</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0.0370633602142334</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0.09760618209838867</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.03594970703125</v>
+        <v>0.03596735000610352</v>
       </c>
     </row>
     <row r="10">
@@ -703,25 +614,16 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.8599867820739746</v>
+        <v>0.1259989738464355</v>
       </c>
       <c r="C10" t="n">
-        <v>0.1246757507324219</v>
+        <v>0.04903173446655273</v>
       </c>
       <c r="D10" t="n">
-        <v>0.05199742317199707</v>
+        <v>0.1274092197418213</v>
       </c>
       <c r="E10" t="n">
-        <v>0.1527853012084961</v>
-      </c>
-      <c r="F10" t="n">
-        <v>0.05016684532165527</v>
-      </c>
-      <c r="G10" t="n">
-        <v>0.1371281147003174</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.04836392402648926</v>
+        <v>0.04787683486938477</v>
       </c>
     </row>
     <row r="11">
@@ -746,21 +648,6 @@
         </is>
       </c>
       <c r="E11" t="inlineStr">
-        <is>
-          <t>═━━━━━═</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>═━━━━━═</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>═━━━━━═</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
         <is>
           <t>═━━━━━═</t>
         </is>

</xml_diff>

<commit_message>
Fase of creating new strategy on going.
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,15 +441,20 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>11100=(11111|11111)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
           <t>00111=(11011|11101)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>11100=(11111|11111)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>00111=(11011|11101)</t>
         </is>
@@ -464,11 +469,14 @@
       <c r="B2" t="n">
         <v>0.25</v>
       </c>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -480,12 +488,15 @@
         <v>0.25</v>
       </c>
       <c r="C3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D3" t="n">
         <v>0</v>
       </c>
-      <c r="D3" t="n">
-        <v>0.25</v>
-      </c>
       <c r="E3" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -499,12 +510,15 @@
         <v>0.25</v>
       </c>
       <c r="C4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D4" t="n">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
-        <v>0.25</v>
-      </c>
       <c r="E4" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -515,16 +529,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="E5" t="n">
-        <v>0</v>
+        <v>0.25</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="6">
@@ -553,6 +570,11 @@
           <t>═━━━━━═</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -561,13 +583,16 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.01952672004699707</v>
-      </c>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="n">
-        <v>0.02027297019958496</v>
-      </c>
-      <c r="E7" t="inlineStr"/>
+        <v>0.02100014686584473</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.02008271217346191</v>
+      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="n">
+        <v>0.02014970779418945</v>
+      </c>
+      <c r="F7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -576,16 +601,19 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.2005040645599365</v>
+        <v>0.1882762908935547</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03600215911865234</v>
+        <v>0.1904587745666504</v>
       </c>
       <c r="D8" t="n">
-        <v>0.1984729766845703</v>
+        <v>0.03456354141235352</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0342252254486084</v>
+        <v>0.1996073722839355</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.0331881046295166</v>
       </c>
     </row>
     <row r="9">
@@ -595,16 +623,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.09668254852294922</v>
+        <v>0.1299138069152832</v>
       </c>
       <c r="C9" t="n">
-        <v>0.03748154640197754</v>
+        <v>0.09871888160705566</v>
       </c>
       <c r="D9" t="n">
-        <v>0.09663057327270508</v>
+        <v>0.03614091873168945</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03596735000610352</v>
+        <v>0.09358668327331543</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.03635573387145996</v>
       </c>
     </row>
     <row r="10">
@@ -614,16 +645,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1259989738464355</v>
+        <v>4.855859518051147</v>
       </c>
       <c r="C10" t="n">
-        <v>0.04903173446655273</v>
+        <v>0.1205987930297852</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1274092197418213</v>
+        <v>0.04657077789306641</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04787683486938477</v>
+        <v>0.1291520595550537</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.04761123657226562</v>
       </c>
     </row>
     <row r="11">
@@ -648,6 +682,11 @@
         </is>
       </c>
       <c r="E11" t="inlineStr">
+        <is>
+          <t>═━━━━━═</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
         <is>
           <t>═━━━━━═</t>
         </is>

</xml_diff>

<commit_message>
Frank Mechthild algorithm implemented without submodularity.
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,6 +449,91 @@
           <t>AbCdEfGhIjKlMnO=(ACMO|AEKO)</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(ACGIMO|AEKO)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(ACEKMO|AEKO)</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|AO)</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|ACMO)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|ACMO)</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|ACGIMO)</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|ACEKMO)</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AO|AEKO)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(ACMO|AEKO)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(ACMO|AEKO)</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(ACGIMO|AEKO)</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(ACEKMO|AEKO)</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|AO)</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|ACMO)</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|ACMO)</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|ACGIMO)</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>AbCdEfGhIjKlMnO=(AEKO|ACEKMO)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
@@ -457,13 +542,64 @@
         </is>
       </c>
       <c r="B2" t="n">
+        <v>1.2e-05</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.2e-05</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1.2e-05</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1.2e-05</v>
+      </c>
+      <c r="F2" t="n">
+        <v>1.2e-05</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.000164</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.000107</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.000107</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.000149</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.000149</v>
+      </c>
+      <c r="L2" t="n">
         <v>0.031722</v>
       </c>
-      <c r="C2" t="n">
+      <c r="M2" t="n">
         <v>0.003815</v>
       </c>
-      <c r="D2" t="n">
+      <c r="N2" t="n">
         <v>0.003815</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.002056</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.001463</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.000316</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.000101</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.000101</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.018506</v>
+      </c>
+      <c r="U2" t="n">
+        <v>0.003008</v>
       </c>
     </row>
     <row r="3">
@@ -473,118 +609,677 @@
         </is>
       </c>
       <c r="B3" t="n">
+        <v>1.2e-05</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1.200000000088818e-05</v>
+      </c>
+      <c r="D3" t="n">
+        <v>1.200000000088818e-05</v>
+      </c>
+      <c r="E3" t="n">
+        <v>1.200002400466294e-05</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.200002400266454e-05</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0.0001640000000008882</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.0001070000000022205</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.0001070000000022205</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.0001500000000017764</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.0001500000000008882</v>
+      </c>
+      <c r="L3" t="n">
         <v>0.03172200000000045</v>
       </c>
-      <c r="C3" t="n">
+      <c r="M3" t="n">
         <v>0.003814000000000891</v>
       </c>
-      <c r="D3" t="n">
+      <c r="N3" t="n">
         <v>0.003814000000000891</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.002053004106001333</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.001461002922</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.0003159999999999998</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.0001010000000008882</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.0001010000000008882</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.01850500000000134</v>
+      </c>
+      <c r="U3" t="n">
+        <v>0.003006000000001778</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>φ Genético</t>
+          <t>φ Stoer-Wagner</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.0005939994060003331</v>
+        <v>0.001481</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0005939994060003331</v>
+        <v>0.003169000000003109</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0005939994060003331</v>
+        <v>0.003169000000003109</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.002911005822007328</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.003010006020007329</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.0003980000000004441</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.003172000000003996</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.003172000000003996</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.001736000000000444</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.004851000000001332</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.03236000000000045</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.03801000000000625</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.03801000000000625</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.01289302578601067</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.01802903605800534</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.003598000000002664</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.009145000000000444</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.009145000000000444</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.02299600000000267</v>
+      </c>
+      <c r="U4" t="n">
+        <v>0.01932100000000889</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>═━━━━═</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>═━━━━═</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>═━━━━═</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>═━━━━═</t>
-        </is>
+          <t>φ Genético</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1.2e-05</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1.200000000088818e-05</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1.200000000088818e-05</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1.200002400466294e-05</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.200002400266454e-05</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0.0001640000000008882</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.0001070000000022205</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.0001070000000022205</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.0001500000000017764</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.0001500000000008882</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.03172200000000045</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.003814000000000891</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.003814000000000891</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.002053004106001333</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.001461002922</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.0003159999999999998</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.0001010000000008882</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.0001010000000008882</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.01850500000000134</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.003006000000001778</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>(ms) PyPhi</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>0.03800034523010254</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0.05600309371948242</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.05800437927246094</v>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="P6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="U6" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>(ms) Fuerza Brutal</t>
+          <t>(ms) PyPhi</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.391458988189697</v>
+        <v>0.05096626281738281</v>
       </c>
       <c r="C7" t="n">
-        <v>2.813121557235718</v>
+        <v>0.0885169506072998</v>
       </c>
       <c r="D7" t="n">
-        <v>3.197590589523315</v>
+        <v>0.05501198768615723</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.15799880027771</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.1355915069580078</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0.03901386260986328</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.05300354957580566</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.05499887466430664</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.1309983730316162</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.1340022087097168</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.03600287437438965</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.05399870872497559</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.05099892616271973</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.1255178451538086</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.1149997711181641</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.04199719429016113</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.06699967384338379</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.05999588966369629</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.1175165176391602</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.1350007057189941</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>(ms) Genético</t>
+          <t>(ms) Fuerza Brutal</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1.43021821975708</v>
+        <v>1.507232189178467</v>
       </c>
       <c r="C8" t="n">
-        <v>2.916515827178955</v>
+        <v>3.102314710617065</v>
       </c>
       <c r="D8" t="n">
-        <v>2.79417896270752</v>
+        <v>2.936008453369141</v>
+      </c>
+      <c r="E8" t="n">
+        <v>12.21799325942993</v>
+      </c>
+      <c r="F8" t="n">
+        <v>12.78816890716553</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1.473705291748047</v>
+      </c>
+      <c r="H8" t="n">
+        <v>3.046900749206543</v>
+      </c>
+      <c r="I8" t="n">
+        <v>2.978136539459229</v>
+      </c>
+      <c r="J8" t="n">
+        <v>22.2933189868927</v>
+      </c>
+      <c r="K8" t="n">
+        <v>23.79830431938171</v>
+      </c>
+      <c r="L8" t="n">
+        <v>1.475276470184326</v>
+      </c>
+      <c r="M8" t="n">
+        <v>3.04181957244873</v>
+      </c>
+      <c r="N8" t="n">
+        <v>2.910391569137573</v>
+      </c>
+      <c r="O8" t="n">
+        <v>12.77681517601013</v>
+      </c>
+      <c r="P8" t="n">
+        <v>13.10311651229858</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>1.554194211959839</v>
+      </c>
+      <c r="R8" t="n">
+        <v>3.302978038787842</v>
+      </c>
+      <c r="S8" t="n">
+        <v>2.968873977661133</v>
+      </c>
+      <c r="T8" t="n">
+        <v>22.5196807384491</v>
+      </c>
+      <c r="U8" t="n">
+        <v>23.03574228286743</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>═━━━━═</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>═━━━━═</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>═━━━━═</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
+          <t>(ms) Stoer-Wagner</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>1.461385488510132</v>
+      </c>
+      <c r="C9" t="n">
+        <v>1.596494913101196</v>
+      </c>
+      <c r="D9" t="n">
+        <v>1.581249713897705</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.948529481887817</v>
+      </c>
+      <c r="F9" t="n">
+        <v>2.264059066772461</v>
+      </c>
+      <c r="G9" t="n">
+        <v>1.405779600143433</v>
+      </c>
+      <c r="H9" t="n">
+        <v>1.5904221534729</v>
+      </c>
+      <c r="I9" t="n">
+        <v>1.674099206924438</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.664482355117798</v>
+      </c>
+      <c r="K9" t="n">
+        <v>2.780578851699829</v>
+      </c>
+      <c r="L9" t="n">
+        <v>1.375328063964844</v>
+      </c>
+      <c r="M9" t="n">
+        <v>1.774580240249634</v>
+      </c>
+      <c r="N9" t="n">
+        <v>1.645856380462646</v>
+      </c>
+      <c r="O9" t="n">
+        <v>2.014770269393921</v>
+      </c>
+      <c r="P9" t="n">
+        <v>2.216013669967651</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1.410415887832642</v>
+      </c>
+      <c r="R9" t="n">
+        <v>1.676884174346924</v>
+      </c>
+      <c r="S9" t="n">
+        <v>1.615114212036133</v>
+      </c>
+      <c r="T9" t="n">
+        <v>2.756566762924194</v>
+      </c>
+      <c r="U9" t="n">
+        <v>2.665369272232056</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>(ms) Genético</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>2.73883843421936</v>
+      </c>
+      <c r="C10" t="n">
+        <v>10.83892917633057</v>
+      </c>
+      <c r="D10" t="n">
+        <v>12.15682435035706</v>
+      </c>
+      <c r="E10" t="n">
+        <v>18.64237141609192</v>
+      </c>
+      <c r="F10" t="n">
+        <v>17.79866600036621</v>
+      </c>
+      <c r="G10" t="n">
+        <v>2.793100595474243</v>
+      </c>
+      <c r="H10" t="n">
+        <v>22.43154907226562</v>
+      </c>
+      <c r="I10" t="n">
+        <v>19.96498250961304</v>
+      </c>
+      <c r="J10" t="n">
+        <v>33.27677488327026</v>
+      </c>
+      <c r="K10" t="n">
+        <v>118.1092202663422</v>
+      </c>
+      <c r="L10" t="n">
+        <v>12.12715721130371</v>
+      </c>
+      <c r="M10" t="n">
+        <v>11.72825169563293</v>
+      </c>
+      <c r="N10" t="n">
+        <v>11.41482067108154</v>
+      </c>
+      <c r="O10" t="n">
+        <v>47.0369131565094</v>
+      </c>
+      <c r="P10" t="n">
+        <v>18.89281225204468</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>2.264527797698975</v>
+      </c>
+      <c r="R10" t="n">
+        <v>11.33360052108765</v>
+      </c>
+      <c r="S10" t="n">
+        <v>11.46251010894775</v>
+      </c>
+      <c r="T10" t="n">
+        <v>43.6169126033783</v>
+      </c>
+      <c r="U10" t="n">
+        <v>50.46710467338562</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
         <is>
           <t>═━━━━═</t>
         </is>

</xml_diff>

<commit_message>
Creating branch for testing.
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -529,7 +529,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.06718897819519043</v>
+        <v>0.0689997673034668</v>
       </c>
     </row>
     <row r="11">
@@ -539,7 +539,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.153458595275879</v>
+        <v>2.229520082473755</v>
       </c>
     </row>
     <row r="12">
@@ -549,7 +549,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.379575252532959</v>
+        <v>0.376002311706543</v>
       </c>
     </row>
     <row r="13">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.6963090896606445</v>
+        <v>1.203050374984741</v>
       </c>
     </row>
     <row r="14">
@@ -569,7 +569,7 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1307392120361328</v>
+        <v>0.1419992446899414</v>
       </c>
     </row>
     <row r="15">
@@ -579,7 +579,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.2574880123138428</v>
+        <v>0.2649993896484375</v>
       </c>
     </row>
     <row r="16">
@@ -589,7 +589,7 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.2002830505371094</v>
+        <v>0.215998649597168</v>
       </c>
     </row>
     <row r="17">

</xml_diff>

<commit_message>
Implemented profiling backend update.
</commit_message>
<xml_diff>
--- a/data/reports/reporte_metricas.xlsx
+++ b/data/reports/reporte_metricas.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="10000=Red de 05 Nodos" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="10000000=Red de 08 Nodos" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>ABCde=(ABC|ABC)</t>
+          <t>ABCDEFGH=(ABCDEFGH|ABCDEFGH)</t>
         </is>
       </c>
     </row>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -457,7 +457,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.24999975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -467,7 +467,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.24999975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -477,7 +477,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.24999975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -487,7 +487,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.24999975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -497,108 +497,88 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.24999975</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>φ Fuerza Brutal</t>
-        </is>
-      </c>
-      <c r="B8" t="n">
-        <v>0.24999975</v>
+          <t>═━━━━═</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>═━━━━═</t>
+        </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>═━━━━═</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>═━━━━═</t>
-        </is>
+          <t>(ms) PyPhi</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.04808282852172852</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>(ms) PyPhi</t>
+          <t>(ms) QRNodes</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.0689997673034668</v>
+        <v>1260.479565143585</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>(ms) QRNodes</t>
+          <t>(ms) QREdges</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>2.229520082473755</v>
+        <v>166.4057974815369</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>(ms) QREdges</t>
+          <t>(ms) Genético</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.376002311706543</v>
+        <v>69.00500822067261</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>(ms) Genético</t>
+          <t>(ms) Stoer-Wagner</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1.203050374984741</v>
+        <v>25.3839955329895</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>(ms) Stoer-Wagner</t>
+          <t>(ms) Ramificación</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.1419992446899414</v>
+        <v>25.20000004768372</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>(ms) Ramificación</t>
-        </is>
-      </c>
-      <c r="B15" t="n">
-        <v>0.2649993896484375</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="1" t="inlineStr">
-        <is>
-          <t>(ms) Fuerza Brutal</t>
-        </is>
-      </c>
-      <c r="B16" t="n">
-        <v>0.215998649597168</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="1" t="inlineStr">
-        <is>
           <t>═━━━━═</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>═━━━━═</t>
         </is>

</xml_diff>